<commit_message>
typo fixed, C1 Value Eagle, Add ALPS files
</commit_message>
<xml_diff>
--- a/PCB/V1.4 Bourns/AtoVproject 16n V1.4 Bourns BOM.xlsx
+++ b/PCB/V1.4 Bourns/AtoVproject 16n V1.4 Bourns BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthwork\Google Drive\eagle online\16n AtoV rework\V1.4 Bourns\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthwork\OneDrive\Documents\GitHub\16n-AtoVproject-rework\PCB\V1.4 Bourns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DD26C5-F948-4C9A-B05F-AC372C5AD101}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A68C972-7872-463D-9564-63105BA14F59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,6 +384,99 @@
     <t xml:space="preserve">	621-1N5819HW-F</t>
   </si>
   <si>
+    <t>Indicate power on state</t>
+  </si>
+  <si>
+    <t>863-NCS20074DR2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	709-SPU01L-12</t>
+  </si>
+  <si>
+    <t>Converts 5V USB to 12V</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Through hole part Use low profile cap</t>
+  </si>
+  <si>
+    <t>604-WP710A10SRC/E</t>
+  </si>
+  <si>
+    <t>tested with 10k-Value shouldn't matter</t>
+  </si>
+  <si>
+    <t>810-CGA3E1X7R1C105AC</t>
+  </si>
+  <si>
+    <t>810-CGA3E2X7R1H104K</t>
+  </si>
+  <si>
+    <t>810-CGA3E2X7R1H103K</t>
+  </si>
+  <si>
+    <t>810-C1608X6S0G106M</t>
+  </si>
+  <si>
+    <t>80-ESS476M025AE2EA</t>
+  </si>
+  <si>
+    <t>603-RT0603FRE074K7L</t>
+  </si>
+  <si>
+    <t>474-DEV-13736</t>
+  </si>
+  <si>
+    <t>Standoff 10mm</t>
+  </si>
+  <si>
+    <t>40 pin Headers to cu to size</t>
+  </si>
+  <si>
+    <t>571-41037410</t>
+  </si>
+  <si>
+    <t>710-970100321</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>652-PTA60432015DPB10</t>
+  </si>
+  <si>
+    <t>D1, D6</t>
+  </si>
+  <si>
+    <t>Standoff 22mm</t>
+  </si>
+  <si>
+    <t>8 position DIP switch</t>
+  </si>
+  <si>
+    <t>S1, S2</t>
+  </si>
+  <si>
+    <t>774-2198MST</t>
+  </si>
+  <si>
+    <t>710-970220361</t>
+  </si>
+  <si>
+    <t>M3 screw</t>
+  </si>
+  <si>
+    <t>M3 countersunk screw</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Diodes - </t>
     </r>
@@ -396,101 +489,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Carefule these are polarised</t>
+      <t>Careful these are polarised</t>
     </r>
-  </si>
-  <si>
-    <t>Indicate power on state</t>
-  </si>
-  <si>
-    <t>863-NCS20074DR2G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	709-SPU01L-12</t>
-  </si>
-  <si>
-    <t>Converts 5V USB to 12V</t>
-  </si>
-  <si>
-    <t>10u</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>Through hole part Use low profile cap</t>
-  </si>
-  <si>
-    <t>604-WP710A10SRC/E</t>
-  </si>
-  <si>
-    <t>tested with 10k-Value shouldn't matter</t>
-  </si>
-  <si>
-    <t>810-CGA3E1X7R1C105AC</t>
-  </si>
-  <si>
-    <t>810-CGA3E2X7R1H104K</t>
-  </si>
-  <si>
-    <t>810-CGA3E2X7R1H103K</t>
-  </si>
-  <si>
-    <t>810-C1608X6S0G106M</t>
-  </si>
-  <si>
-    <t>80-ESS476M025AE2EA</t>
-  </si>
-  <si>
-    <t>603-RT0603FRE074K7L</t>
-  </si>
-  <si>
-    <t>474-DEV-13736</t>
-  </si>
-  <si>
-    <t>Standoff 10mm</t>
-  </si>
-  <si>
-    <t>40 pin Headers to cu to size</t>
-  </si>
-  <si>
-    <t>571-41037410</t>
-  </si>
-  <si>
-    <t>710-970100321</t>
-  </si>
-  <si>
-    <t>Bourns</t>
-  </si>
-  <si>
-    <t>652-PTA60432015DPB10</t>
-  </si>
-  <si>
-    <t>D1, D6</t>
-  </si>
-  <si>
-    <t>Standoff 22mm</t>
-  </si>
-  <si>
-    <t>8 position DIP switch</t>
-  </si>
-  <si>
-    <t>S1, S2</t>
-  </si>
-  <si>
-    <t>774-2198MST</t>
-  </si>
-  <si>
-    <t>710-970220361</t>
-  </si>
-  <si>
-    <t>M3 screw</t>
-  </si>
-  <si>
-    <t>M3 countersunk screw</t>
   </si>
 </sst>
 </file>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9296875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1689,7 +1689,7 @@
         <v>23</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>91</v>
@@ -1712,13 +1712,13 @@
         <v>70</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1746,13 +1746,13 @@
         <v>17</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -1775,7 +1775,7 @@
         <v>19</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
@@ -1798,7 +1798,7 @@
         <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
@@ -1806,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>16</v>
@@ -1815,13 +1815,13 @@
         <v>17</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
@@ -1844,15 +1844,15 @@
         <v>38</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1875,7 +1875,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>8</v>
@@ -1929,10 +1929,10 @@
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>98</v>
@@ -2050,10 +2050,10 @@
         <v>47</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
@@ -2184,20 +2184,20 @@
         <v>2</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
@@ -2241,23 +2241,23 @@
         <v>74</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E38" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E39" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
@@ -2265,7 +2265,7 @@
         <v>12</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
@@ -2273,7 +2273,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
@@ -2281,10 +2281,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>